<commit_message>
Project Risks and Cover Added
</commit_message>
<xml_diff>
--- a/Risk Register.xlsx
+++ b/Risk Register.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSSPM\Semester3\Practicum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC65BFE-2972-4E47-A8D2-CEE5D0F5E005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628AEFBA-34B4-46BA-BF4A-6F0E1084AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
   <si>
     <t>Description of Potential Risk</t>
   </si>
@@ -202,15 +202,6 @@
     <t>Temporarily disable news feature, inform users.</t>
   </si>
   <si>
-    <t>Usability</t>
-  </si>
-  <si>
-    <t>Conduct usability testing with novice traders, apply responsive design principles.</t>
-  </si>
-  <si>
-    <t>Release UI fixes in hotpatch update.</t>
-  </si>
-  <si>
     <t>External Broker Dependency</t>
   </si>
   <si>
@@ -241,12 +232,6 @@
     <t>Users may not get updated news, lowering trust.</t>
   </si>
   <si>
-    <t>Poor Usability</t>
-  </si>
-  <si>
-    <t>Users may abandon bot due to bad UX.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Risk Rating </t>
   </si>
   <si>
@@ -260,6 +245,126 @@
   </si>
   <si>
     <t>50+</t>
+  </si>
+  <si>
+    <t>Additional unplanned features may delay timeline and increase costs.</t>
+  </si>
+  <si>
+    <t>Clearly define scope, enforce change control process.</t>
+  </si>
+  <si>
+    <t>Negotiate revised timeline or descoped deliverables.</t>
+  </si>
+  <si>
+    <t>Bi-weekly Sprint Review</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Resource Shortage</t>
+  </si>
+  <si>
+    <t>Unavailability of key developers or testers delays project.</t>
+  </si>
+  <si>
+    <t>Resource backup planning, cross-training team members.</t>
+  </si>
+  <si>
+    <t>Hire contractors or outsource temporarily.</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Budget Overrun</t>
+  </si>
+  <si>
+    <t>Costs may exceed allocated budget.</t>
+  </si>
+  <si>
+    <t>Strict financial monitoring, milestone-based payments.</t>
+  </si>
+  <si>
+    <t>Request additional budget approval or descale features.</t>
+  </si>
+  <si>
+    <t>Technology Integration Failure</t>
+  </si>
+  <si>
+    <t>Integration with MT5 API or other services may fail.</t>
+  </si>
+  <si>
+    <t>Early prototyping, POC testing.</t>
+  </si>
+  <si>
+    <t>Switch to alternate APIs or delay integration.</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Timeline Delays</t>
+  </si>
+  <si>
+    <t>Project not delivered on agreed schedule.</t>
+  </si>
+  <si>
+    <t>Use Agile sprints, track with project management tools.</t>
+  </si>
+  <si>
+    <t>Re-baseline project plan, inform stakeholders.</t>
+  </si>
+  <si>
+    <t>Bi-weekly</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Knowledge Gap</t>
+  </si>
+  <si>
+    <t>Team lacks expertise in MT5, trading, or security.</t>
+  </si>
+  <si>
+    <t>Provide training, hire domain experts.</t>
+  </si>
+  <si>
+    <t>Engage external consultants if required.</t>
+  </si>
+  <si>
+    <t>Communication Breakdown</t>
+  </si>
+  <si>
+    <t>Miscommunication between stakeholders delays decision-making.</t>
+  </si>
+  <si>
+    <t>Weekly standups, project status reports.</t>
+  </si>
+  <si>
+    <t>Escalate to project sponsor for alignment.</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Vendor/Third-party Dependency</t>
+  </si>
+  <si>
+    <t>Delay or failure from vendors (e.g., hosting, MT5 services).</t>
+  </si>
+  <si>
+    <t>SLA agreements, multiple vendors.</t>
+  </si>
+  <si>
+    <t>Switch vendor or fallback plan.</t>
+  </si>
+  <si>
+    <t>Project Scope Creep</t>
   </si>
 </sst>
 </file>
@@ -316,12 +421,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,9 +494,469 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>396241</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1089661</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>172085</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Freeform 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B174B7F9-4A27-051B-C4D7-68DD35790217}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="396241" y="342900"/>
+          <a:ext cx="693420" cy="377825"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="798480" h="416208">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="798480" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="798480" y="416208"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="416208"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+        <a:ln cap="sq">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>131194</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB434D3-DC23-2D20-9F39-2E350D10A079}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="198120" y="396240"/>
+          <a:ext cx="8176260" cy="466474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="70000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="800"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="4000" b="1" kern="1200" spc="-145">
+              <a:solidFill>
+                <a:srgbClr val="0B76A0"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="Manrope Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Automated Crypto Trading Bot</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1531620</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A779D3-4EEF-7F1A-E32B-CF0F8C3E7C39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="899160"/>
+          <a:ext cx="4236720" cy="528320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1" kern="1200">
+              <a:solidFill>
+                <a:srgbClr val="10282A">
+                  <a:alpha val="68000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Risk Register</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1783080</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4511040</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC2999D-6E48-94E6-E48E-2C22C47B410F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9189720" y="815340"/>
+          <a:ext cx="2727960" cy="1021080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="70000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="800"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" kern="1200" spc="-145">
+              <a:solidFill>
+                <a:srgbClr val="244061"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="Manrope Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Syed Waqar Ali	24k-8301</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050" b="0" kern="0" spc="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="70000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="800"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" kern="1200" spc="-145">
+              <a:solidFill>
+                <a:srgbClr val="244061"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="Manrope Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Mohammad. Mustansir	24k-8305</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="70000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="800"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" kern="1200" spc="-145">
+              <a:solidFill>
+                <a:srgbClr val="244061"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="Manrope Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Asad		24k-8324</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1050">
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1592580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4465320</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067DDDCE-EB38-CFD1-78F0-87E285B9D96E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8999220" y="350520"/>
+          <a:ext cx="2872740" cy="312420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0E2841">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="70000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="800"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="1000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" kern="1200" spc="-145">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Manrope"/>
+              <a:ea typeface="Manrope Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Presented By</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="900">
+            <a:effectLst/>
+            <a:latin typeface="Cambria" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+            <a:ea typeface="MS Mincho" panose="02020609040205080304" pitchFamily="49" charset="-128"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C113782-5BE2-417F-B437-1EAC24A5DA44}" name="Table1" displayName="Table1" ref="A1:K12" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:K12" xr:uid="{5C113782-5BE2-417F-B437-1EAC24A5DA44}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5C113782-5BE2-417F-B437-1EAC24A5DA44}" name="Table1" displayName="Table1" ref="A12:K30" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A12:K30" xr:uid="{5C113782-5BE2-417F-B437-1EAC24A5DA44}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C55034E8-FCB2-4AF1-A783-4227D0500B59}" name="Description of Potential Risk"/>
     <tableColumn id="2" xr3:uid="{F3C045F4-DC16-4D98-9136-45148A42C912}" name="Description of Potential Impact"/>
@@ -404,8 +975,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{55AF9EDD-5C0B-4CF2-B59A-13E67084ACAE}" name="Table2" displayName="Table2" ref="A15:B19" totalsRowShown="0">
-  <autoFilter ref="A15:B19" xr:uid="{55AF9EDD-5C0B-4CF2-B59A-13E67084ACAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{55AF9EDD-5C0B-4CF2-B59A-13E67084ACAE}" name="Table2" displayName="Table2" ref="A35:B39" totalsRowShown="0">
+  <autoFilter ref="A35:B39" xr:uid="{55AF9EDD-5C0B-4CF2-B59A-13E67084ACAE}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8074821D-CE5F-460D-B17A-320671133D5A}" name="Risk Rating "/>
     <tableColumn id="2" xr3:uid="{88ED110E-6F16-455C-AD42-83854F8DAEF9}" name="Priority"/>
@@ -701,493 +1272,889 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="68.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.5546875" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D13" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="F2">
+      <c r="F13">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="G13">
         <v>4</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J13" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E14" t="s">
         <v>26</v>
       </c>
-      <c r="F3">
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="G14">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J14" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="H15">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="I15">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J15" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E16" t="s">
         <v>28</v>
       </c>
-      <c r="F5">
+      <c r="F16">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G16">
         <v>3</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J16" t="s">
         <v>32</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D17" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E17" t="s">
         <v>25</v>
       </c>
-      <c r="F6">
+      <c r="F17">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="G17">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J17" t="s">
         <v>33</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D18" t="s">
         <v>53</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
+      <c r="F18">
         <v>4</v>
       </c>
-      <c r="G7">
+      <c r="G18">
         <v>4</v>
       </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J18" t="s">
         <v>34</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B20" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
+      <c r="F20">
         <v>4</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="3">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>24</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>5</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2</v>
+      </c>
+      <c r="I24" s="3">
+        <v>30</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2</v>
+      </c>
+      <c r="I25" s="3">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="3">
+        <v>3</v>
+      </c>
+      <c r="G26" s="3">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>30</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3</v>
+      </c>
+      <c r="G27" s="3">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3">
+        <v>24</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3">
+        <v>16</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="3">
+        <v>3</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2</v>
+      </c>
+      <c r="I29" s="3">
+        <v>18</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3">
+        <v>5</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2</v>
+      </c>
+      <c r="I30" s="3">
+        <v>20</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K30" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>60</v>
-      </c>
-      <c r="J9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <v>12</v>
-      </c>
-      <c r="J11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="22" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>